<commit_message>
GreenKart End to End
</commit_message>
<xml_diff>
--- a/GreenKartAutomation.xlsx
+++ b/GreenKartAutomation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/2119444_cognizant_com/Documents/Documents/EclipseWorkSpace/Framework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{9BCCBD30-E924-4CAB-9E50-FCF0CD5A9059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35ADABFA-A7D9-4EB8-9550-A8C578FF8593}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="8_{9BCCBD30-E924-4CAB-9E50-FCF0CD5A9059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCF15D84-ABA7-4AAE-B196-606A88D57822}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{49EFC985-6292-4A6E-A627-2EE01EB0100F}"/>
   </bookViews>
@@ -41,24 +41,12 @@
     <t>TestCaseNames</t>
   </si>
   <si>
-    <t>Vegetablekart</t>
-  </si>
-  <si>
-    <t>FruitsCart</t>
-  </si>
-  <si>
     <t>Vegetables</t>
   </si>
   <si>
     <t>Fruits</t>
   </si>
   <si>
-    <t>Onion,Cucumber,Brocolli</t>
-  </si>
-  <si>
-    <t>3,2,2</t>
-  </si>
-  <si>
     <t>Apple,Banana,Mango</t>
   </si>
   <si>
@@ -69,19 +57,37 @@
   </si>
   <si>
     <t>FruitsQTY</t>
+  </si>
+  <si>
+    <t>orderVegetables</t>
+  </si>
+  <si>
+    <t>orderFruits</t>
+  </si>
+  <si>
+    <t>Onion,Cucumber,Brocolli,Musk Melon</t>
+  </si>
+  <si>
+    <t>3,2,2,10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -119,9 +125,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,7 +448,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -455,42 +464,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
+      <c r="A2" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>